<commit_message>
DSP OpenCV Car 3 developped but still not working
</commit_message>
<xml_diff>
--- a/DSP/Task9/changelog.xlsx
+++ b/DSP/Task9/changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - Politechnika Wroclawska\Pulpit\AAE\DSP\Task9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E81E3-C7A1-4478-96E3-A2C90C2A10EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F50558C-C0DF-466B-BC6C-3947EE134DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,15 +266,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>11351</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>163751</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -297,8 +297,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6943725" y="1695451"/>
-          <a:ext cx="1743075" cy="1363900"/>
+          <a:off x="7000875" y="1657351"/>
+          <a:ext cx="1743075" cy="1173400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -664,7 +664,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>